<commit_message>
working on phase 2
</commit_message>
<xml_diff>
--- a/resources/import/company_invoice.xlsx
+++ b/resources/import/company_invoice.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>رقم الفاتورة</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>بنك</t>
-  </si>
-  <si>
-    <t xml:space="preserve">اذن صرف عمولة </t>
   </si>
 </sst>
 </file>
@@ -140,7 +137,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border/>
     <border>
       <left style="medium">
@@ -177,19 +174,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
     </border>
     <border>
       <left style="medium">
@@ -237,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -247,7 +231,6 @@
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="2" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -267,33 +250,54 @@
     <xf borderId="3" fillId="0" fontId="5" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="16" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="16" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="6" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="16" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="2" vertical="center"/>
     </xf>
+    <xf borderId="5" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="2" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="8" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="7" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="2" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="4" fontId="8" numFmtId="4" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="9" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -570,102 +574,104 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="3" t="str">
-        <f t="shared" ref="O1:O3" si="1">CONCATENATE(Q1,G1)</f>
-        <v>اذن صرف عمولة رقم إذن العمولة</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="O2" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>اذن صرف عمولة </v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="Q2" s="3"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="O3" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>اذن صرف عمولة </v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="19"/>
       <c r="I4" s="20"/>
       <c r="J4" s="21"/>
       <c r="K4" s="20"/>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
-      <c r="Q4" s="4"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="26">
-        <f t="shared" ref="I5:K5" si="2">SUM(I2:I3)</f>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28">
+        <f t="shared" ref="I5:K5" si="1">SUM(I2:I3)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="26">
-        <f t="shared" si="2"/>
+      <c r="J5" s="28">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K5" s="26">
-        <f t="shared" si="2"/>
+      <c r="K5" s="28">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L5" s="24"/>
-      <c r="M5" s="27"/>
-      <c r="O5" s="3" t="str">
-        <f>CONCATENATE(Q5,G5)</f>
-        <v>اذن صرف عمولة </v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="L5" s="26"/>
+      <c r="M5" s="29"/>
+      <c r="Q5" s="3"/>
     </row>
     <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1"/>

</xml_diff>